<commit_message>
Cadastro de aluno por upload e outros serviços
</commit_message>
<xml_diff>
--- a/src/backend/tests/lista_alunos.xlsx
+++ b/src/backend/tests/lista_alunos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisGuilhermeGaboard\06_AcompanhamentoEnsinoMedio\src\backend\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisGuilhermeGaboard\06_AcompanhamentoEnsinoMedio\src\backend\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1DA1B-9B14-4201-B016-83FE20F05946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0AB4D8-BF43-4747-8F3C-4A4A086B7C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1875" windowWidth="14445" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Inness Hambatch</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>rua 5437</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>78502938</t>
+  </si>
+  <si>
+    <t>68409712</t>
   </si>
 </sst>
 </file>
@@ -139,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +474,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -520,11 +536,11 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>39872</v>
+      <c r="A2" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>7241</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -541,7 +557,7 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>70507</v>
       </c>
       <c r="I2" t="s">
@@ -556,22 +572,22 @@
       <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="b">
-        <v>0</v>
+      <c r="M2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>35111</v>
+      <c r="A3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>6902</v>
+        <v>437</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -582,7 +598,7 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>79048</v>
       </c>
       <c r="I3" t="s">
@@ -597,8 +613,8 @@
       <c r="L3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="b">
-        <v>0</v>
+      <c r="M3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>